<commit_message>
update of 3 property numbers
</commit_message>
<xml_diff>
--- a/property/S72.xlsx
+++ b/property/S72.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\business\property\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14B855E0-4DF6-41B4-9CBB-917CCF4B39F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331C267D-8492-4282-89A3-4A7DA3D5F549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-285" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{7D85F463-FDA3-4EC2-B3ED-40B94F1D36DF}"/>
   </bookViews>
@@ -902,7 +902,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>